<commit_message>
ajustes finais. front, ml, transformaçao para meses, imagem apenas em local. pfv nao quebre
</commit_message>
<xml_diff>
--- a/static/scraped_data.xlsx
+++ b/static/scraped_data.xlsx
@@ -482,462 +482,470 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Bicicleta Aro 29 Ksw 21 Marchas Shimano Freio Hidraulico</t>
+          <t>Kit Composteira Doméstica / Minhocário G + Minhocas - 60l Sf</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1.789</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr"/>
+          <t>397</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Por Casologica</t>
+        </is>
+      </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>4.5</t>
+          <t>4.7</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G2" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Kit Bateria Painel Solar 3 Lâmpadas Poste Prova D'água Led</t>
+          <t>Coletor Menstrual Korui - Pôr Do Sol</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>209</t>
+          <t>79</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>4.9</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G3" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Bicicleta Aro 29 Ksw 21 Marchas Shimano Freio Hidraulico</t>
+          <t>Carbo 100% Natural Mombora - Kit 4 Sachês - Variados</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1.789</t>
+          <t>42</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
-          <t>4.5</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G4" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Placa Solar Painel Solar 150w + Manual</t>
+          <t>Escova De Dentes Bambu Ecológica Sustentável Biodegradável</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>375</t>
+          <t>13</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>4.3</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G5" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Bicicleta Elétrica Goon.up 500w - 40km/h - Bateria Chumbo.</t>
+          <t>Kit Composteira Doméstica / Minhocário G + Minhocas - 60l Sf</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>5.490</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr"/>
+          <t>397</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Por Casologica</t>
+        </is>
+      </c>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr">
         <is>
-          <t>4.6</t>
+          <t>4.7</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G6" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>KIT 12 Nude Cremoso bebida de aveia 1L</t>
+          <t>Coletor Menstrual Korui - Pôr Do Sol</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>198</t>
+          <t>79</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr">
         <is>
-          <t>4.6</t>
+          <t>4.9</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G7" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Kit 100 Unidades Squeeze 600 Ml Alumínio Personalizado</t>
+          <t xml:space="preserve">Bio2 Barra Protein Vegana Cacau E Maca Peruana Dp Com 12un  </t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2.408</t>
+          <t>189</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>4.6</t>
+        </is>
+      </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G8" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Bicicleta Aro 29 Forss Aluminio 21 Marchas Pneus Faixa Bege</t>
+          <t>Filtro Agua 9 3/4 Ponto De Uso Pou Carvão Ativado Tira Cloro</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>1.249</t>
+          <t>141</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>4.8</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G9" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Fazenda Sao Roque vinagre de maça São Roque 100% orgânico</t>
+          <t>51mm Portafilter Nu Substitua Por Alça Longa Para</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr"/>
+          <t>126</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Por Suntek</t>
+        </is>
+      </c>
       <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>4.9</t>
-        </is>
-      </c>
+      <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G10" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Bicicleta Elétrica  Next Electric®  Distribuidor Oficial </t>
+          <t>Inciclo Coletor Menstrual A + Copinho Esterilizador</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>7.950</t>
+          <t>78</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr">
         <is>
-          <t>4.9</t>
+          <t>4.7</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G11" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Bebida à Base de Castanha-de-Caju e Aveia A Tal da Castanha Barista Profissional Caixa 1l</t>
+          <t>Filtro Refil Purificador De Água Avanti Ibbl Original</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>42</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr">
         <is>
-          <t>4.8</t>
+          <t>4.7</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G12" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H12" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Calça Cargo Masculina Larga Skate Bolso Lateral Unissex Nfe</t>
+          <t>Garrafa De Água Sem Bpa 2500ml À Prova De Vazamentos Jarro</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>67</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr"/>
+          <t>103</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Por Suntek</t>
+        </is>
+      </c>
       <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>4.6</t>
-        </is>
-      </c>
+      <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G13" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H13" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>100 Unidades Squeeze 500ml Plástico</t>
+          <t>Camiseta Personalizada Underflow Malha Ecológica</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>390</t>
+          <t>93</t>
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr">
         <is>
-          <t>4.9</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G14" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H14" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Bicicleta Aro 20 Cross Gtsprint Aro Aero V-brake Bmx</t>
+          <t xml:space="preserve">Cartucho Hp 667xl Preto E 667xl Colorido Original E Lacrado </t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>689</t>
+          <t>188</t>
         </is>
       </c>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr">
         <is>
-          <t>4.5</t>
+          <t>4.1</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G15" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H15" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Moletom Feminino Essentials 3-stripes Com Capuz adidas</t>
+          <t>Garrafa Térmica Aço Inox Água Gelada Garantida Por 24 Horas</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>399</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Por adidas</t>
-        </is>
-      </c>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G16" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H16" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Kit Bateria Painel Solar 3 Lâmpadas Poste Prova D'água Led</t>
+          <t>Filtro De Barro Salute 12 Litros - C/1 Vela C/carvão + Bóia</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>209</t>
+          <t>189</t>
         </is>
       </c>
       <c r="C17" t="inlineStr"/>
@@ -949,359 +957,347 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G17" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H17" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Bebida Vegetal Original Orgânico A Tal da Castanha 1 Litro</t>
+          <t>Leite De Coco Em Pó 1kg -  100% Puro Premium</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>85</t>
         </is>
       </c>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr">
         <is>
-          <t>4.8</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G18" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H18" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Calça Pit Bull Pitbull Pit Bul Jeans 33138</t>
+          <t>2 Coador De Café Algodão Sustentável Reutilizável Melita 103</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>350</t>
+          <t>52</t>
         </is>
       </c>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr">
         <is>
-          <t>4.5</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G19" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H19" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Garrafa Squeeze De Água Para Academia 1l Fitness Promoção</t>
+          <t>Camiseta Johnny Cash Folson Prison Blues Malha Ecológica</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>78</t>
         </is>
       </c>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>4.7</t>
-        </is>
-      </c>
+      <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G20" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H20" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Mountain bike Woltz Steel aro 29 17" 21v freios de disco mecânico câmbios Yamada cor preto/vermelho</t>
+          <t>Camiseta Sonic Youth Dirty Indie Rock Malha Ecológica</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>1.169</t>
+          <t>78</t>
         </is>
       </c>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr">
         <is>
-          <t>4.5</t>
+          <t>4.7</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G21" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H21" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Tapete De Yoga Mat Tpe Estampado Com Bolsa Biodegradável 6mm</t>
+          <t>16 Shampoos E Sabonetes Veganos Da Expresso Mata Atlântica</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>159</t>
+          <t>405</t>
         </is>
       </c>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr">
         <is>
-          <t>4.8</t>
+          <t>4.7</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G22" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H22" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Granola De Cereais Zero Açúcar 1kg - Frutas E Castanhas</t>
+          <t>1 Cápsula Nespresso Recarregável Reutilizável Cafeteira Café</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>46</t>
+          <t>19</t>
         </is>
       </c>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G23" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H23" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Bebida à Base de Aveia Original Naveia Caixa 1l</t>
+          <t xml:space="preserve">Camiseta Soundgarden Badmotorfinger Grunge Chris Cornell </t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>78</t>
         </is>
       </c>
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr">
         <is>
-          <t>4.8</t>
+          <t>4.9</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G24" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H24" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Meias Cushioned Sportswear Ankle 3 Pares adidas</t>
+          <t>Diário Lunar - Primeiros Ciclos Menstruais</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>79</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Por adidas</t>
-        </is>
-      </c>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr"/>
       <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>4.8</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G25" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H25" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Kit 3 Velas Para Massagem Relaxante Arte Dos Aromas 100g</t>
+          <t>4 Saquinhos Reutilizáveis Sustentável Ecológico Legume Fruta</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>201</t>
+          <t>55</t>
         </is>
       </c>
       <c r="C26" t="inlineStr"/>
       <c r="D26" t="inlineStr"/>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>5.0</t>
-        </is>
-      </c>
+      <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G26" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H26" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Bicicleta Infantil Feminina Com Rodinha Aro 20 Bella 2023</t>
+          <t>Calcinha Absorvente Korui - 1 Unidade</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>616</t>
+          <t>89</t>
         </is>
       </c>
       <c r="C27" t="inlineStr"/>
       <c r="D27" t="inlineStr"/>
       <c r="E27" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G27" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H27" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Capsula Nespresso Kit 3un Inox Reutilizável E 1 Tamper Inox</t>
+          <t>600 Unid De Cotonete Madeira Algodão Sustentável Ecológico</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>199</t>
+          <t>139</t>
         </is>
       </c>
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G28" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H28" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Óleo de Coco Extra Virgem Orgânico Copra Vidro 500ml</t>
+          <t>Coletor Menstrual Korui - Amazônia</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>79</t>
         </is>
       </c>
       <c r="C29" t="inlineStr"/>
@@ -1313,501 +1309,493 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G29" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H29" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Kit 12 Nude baunilha leite de aveia 1L</t>
+          <t>Camiseta Rage Against The Machine Evil Empire Malha Eco</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>198</t>
+          <t>78</t>
         </is>
       </c>
       <c r="C30" t="inlineStr"/>
       <c r="D30" t="inlineStr"/>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>4.8</t>
-        </is>
-      </c>
+      <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G30" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H30" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Protetores De Seios Lib Pétalas 4 Pares Bege</t>
+          <t>Cachaça Camponeses Orgânica E Artesanal 700ml - Carvalho</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>78</t>
         </is>
       </c>
       <c r="C31" t="inlineStr"/>
       <c r="D31" t="inlineStr"/>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>4.5</t>
-        </is>
-      </c>
+      <c r="E31" t="inlineStr"/>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G31" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H31" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>5x Fraldinha Boca + 5x Ombro Estampas Safari 100% Algodão</t>
+          <t xml:space="preserve">10 Fraldinhas Boca Bebê 100% Algodão 33x33 Ctms + 1 Brinde </t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>66</t>
+          <t>53</t>
         </is>
       </c>
       <c r="C32" t="inlineStr"/>
       <c r="D32" t="inlineStr"/>
       <c r="E32" t="inlineStr">
         <is>
-          <t>4.3</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G32" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H32" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Bicicleta Aro 29 Gts Alumunio Rdx 21v Câmbio Shimano A Disco Cor Cinza/preto Tamanho Do Quadro 19</t>
+          <t>Vela Sustentável E Vegana 100% Natural De Maracujá</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>1.199</t>
+          <t>39</t>
         </is>
       </c>
       <c r="C33" t="inlineStr"/>
       <c r="D33" t="inlineStr"/>
       <c r="E33" t="inlineStr">
         <is>
-          <t>4.5</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G33" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H33" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Adaptador Capsula Dolce Gusto Genio S- Piccolo + Tamper Inox</t>
+          <t>Horta Vertical- Produto Sustentável</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>179</t>
+          <t>273</t>
         </is>
       </c>
       <c r="C34" t="inlineStr"/>
       <c r="D34" t="inlineStr"/>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>4.6</t>
-        </is>
-      </c>
+      <c r="E34" t="inlineStr"/>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G34" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H34" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Brinquedo Montessori Mecânica Contrutor Ferramentas Infantil</t>
+          <t>Garrafa Squeeze Feita Tritan Certificada - Bpa Free</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>179</t>
+          <t>78</t>
         </is>
       </c>
       <c r="C35" t="inlineStr"/>
       <c r="D35" t="inlineStr"/>
       <c r="E35" t="inlineStr">
         <is>
-          <t>4.4</t>
+          <t>4.9</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G35" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H35" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Leite De Coco Em Pó 100% Puro - 1kg</t>
+          <t>Shampoo Sólido 100% Natural Murumuru, Amêndoa E Mandarina</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>78</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr"/>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Por Insitta</t>
+        </is>
+      </c>
       <c r="D36" t="inlineStr"/>
       <c r="E36" t="inlineStr">
         <is>
-          <t>4.4</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G36" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H36" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Kit 6 Vinagre De Maçã Orgânico Montes Verdes 530ml</t>
+          <t>Cápsula Nespresso Reutilizável Inox + Tamper</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>145</t>
+          <t>139</t>
         </is>
       </c>
       <c r="C37" t="inlineStr"/>
       <c r="D37" t="inlineStr"/>
       <c r="E37" t="inlineStr">
         <is>
-          <t>4.9</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G37" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H37" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Kit 3 Pares Rosquinhas De Peito Seios Amamentação Lavável</t>
+          <t>Kit Full Vidro - 3 Retos + 3 Curvos + Escova - Canudos</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>34</t>
+          <t>32</t>
         </is>
       </c>
       <c r="C38" t="inlineStr"/>
       <c r="D38" t="inlineStr"/>
       <c r="E38" t="inlineStr">
         <is>
-          <t>4.4</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G38" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H38" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Mountain bike Ello Bike Velox aro 29 21v freios de disco mecânico câmbios Ltx cor preto/rosa</t>
+          <t xml:space="preserve"> Painel Jardim Vertical + Irrigação + Impermeabilizante</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>798</t>
+          <t>358</t>
         </is>
       </c>
       <c r="C39" t="inlineStr"/>
       <c r="D39" t="inlineStr"/>
       <c r="E39" t="inlineStr">
         <is>
-          <t>4.3</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G39" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H39" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Squeeze Térmico  Personalizado Seu Nome A Laser</t>
+          <t>Cápsula Nespresso Reutilizável Inox</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>55</t>
         </is>
       </c>
       <c r="C40" t="inlineStr"/>
       <c r="D40" t="inlineStr"/>
       <c r="E40" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G40" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H40" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Notebook Dell Latitude 5490 Intel Core I5 8ªger 8gb 128gb</t>
+          <t>Camiseta Hüsker Dü Husker Du Hardcore Punk Emo Bob Mould</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>1.489</t>
+          <t>78</t>
         </is>
       </c>
       <c r="C41" t="inlineStr"/>
       <c r="D41" t="inlineStr"/>
       <c r="E41" t="inlineStr">
         <is>
-          <t>4.8</t>
+          <t>4.3</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G41" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H41" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>12 Leite Vegetal Bebida Aveia Barista Profissional 1 Litro</t>
+          <t xml:space="preserve">Cumbuca /tigela /bowl De Coco Natural </t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>296</t>
+          <t>29</t>
         </is>
       </c>
       <c r="C42" t="inlineStr"/>
       <c r="D42" t="inlineStr"/>
       <c r="E42" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G42" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H42" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t xml:space="preserve">Pó Mago Para Decoração Pérola 50g </t>
+          <t>Kit Talheres De Bambu - Reutilizáveis - Acompanha Ecobag</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>32</t>
         </is>
       </c>
       <c r="C43" t="inlineStr"/>
       <c r="D43" t="inlineStr"/>
-      <c r="E43" t="inlineStr"/>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>4.5</t>
+        </is>
+      </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G43" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H43" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Conchas Protetoras Para Amamentação Base Silicone Buba Bico</t>
+          <t>Módulo Jardim Vertical + Camada Impermeável + Kit Instalação</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>349</t>
         </is>
       </c>
       <c r="C44" t="inlineStr"/>
       <c r="D44" t="inlineStr"/>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>4.7</t>
-        </is>
-      </c>
+      <c r="E44" t="inlineStr"/>
       <c r="F44" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G44" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H44" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Bicicleta Aro 20 Ksvj Cross Bmx Freestyle Infantil Aero</t>
+          <t>Vela Aromática Perfumada Vegetal Spice Canela</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>899</t>
+          <t>37</t>
         </is>
       </c>
       <c r="C45" t="inlineStr"/>
       <c r="D45" t="inlineStr"/>
       <c r="E45" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>4.4</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G45" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H45" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Kit 2 Velas Aromáticas Perfumada Capim Limão E Lavanda 100gr</t>
+          <t>Capa Pet Dobrável Impermeável Protetor Para Bancos De Carros</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>179</t>
         </is>
       </c>
       <c r="C46" t="inlineStr"/>
@@ -1819,168 +1807,156 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G46" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H46" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Notebook Dell Latitude E5450 Core I5  16 Gb Ram  480 Gb Ssd</t>
+          <t>Caixinha De Som Amplificadora Para Celular Portátil Pinus</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>2.550</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>Por Tech Forte</t>
-        </is>
-      </c>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr"/>
       <c r="D47" t="inlineStr"/>
       <c r="E47" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>4.7</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G47" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H47" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Possible bebida à base de castanha de caju orgânica leite caixa 1L</t>
+          <t>Kit Mochila Kraft + Térmica 500ml Br+ Canudos Inox 6-1 Roxo</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>254</t>
         </is>
       </c>
       <c r="C48" t="inlineStr"/>
       <c r="D48" t="inlineStr"/>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>4.6</t>
-        </is>
-      </c>
+      <c r="E48" t="inlineStr"/>
       <c r="F48" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G48" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H48" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Kit 3 Garrafa Água Academia 2000 900  300ml Squeezes Adesivo</t>
+          <t xml:space="preserve">Garrafa Retrátil Silicone </t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>56</t>
         </is>
       </c>
       <c r="C49" t="inlineStr"/>
       <c r="D49" t="inlineStr"/>
       <c r="E49" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G49" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H49" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Coletor Menstrual Inciclo + Cápsula Esterilizadora</t>
+          <t>Mochila Papel Kraft Impermeável - Compartimento Laptop</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>141</t>
+          <t>199</t>
         </is>
       </c>
       <c r="C50" t="inlineStr"/>
       <c r="D50" t="inlineStr"/>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>4.8</t>
-        </is>
-      </c>
+      <c r="E50" t="inlineStr"/>
       <c r="F50" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G50" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H50" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Vinagre De Maçã Orgânico Fruta Nobre 530ml Montes Verdes</t>
+          <t>Kit 3 Comedouros Pássaros Livres. Garrafa Vinho Branca</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>227</t>
         </is>
       </c>
       <c r="C51" t="inlineStr"/>
       <c r="D51" t="inlineStr"/>
       <c r="E51" t="inlineStr">
         <is>
-          <t>4.8</t>
+          <t>4.4</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-23</t>
         </is>
       </c>
       <c r="G51" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
       <c r="H51" s="2" t="n">
-        <v>45551.73464590661</v>
+        <v>45558.49492337153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>